<commit_message>
Actualizacion de carta inicio 450,000
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Luna\Documents\UAG\Gestion de proyectos\proyecto final\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AC5F58-6214-4EA0-AB89-23701DDBF1AE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B889483-21DB-4030-9888-42438EB697BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="129">
   <si>
     <t>JULIO</t>
   </si>
@@ -38,18 +38,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>JP</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <t>WS</t>
   </si>
   <si>
     <t>WBS</t>
@@ -413,6 +401,15 @@
   </si>
   <si>
     <t>NOV</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>JM</t>
+  </si>
+  <si>
+    <t>IJ</t>
   </si>
 </sst>
 </file>
@@ -985,10 +982,10 @@
   <dimension ref="A1:AI1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1046,20 +1043,20 @@
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
       <c r="M2" s="30" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
       <c r="Q2" s="30"/>
       <c r="R2" s="30" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="S2" s="30"/>
       <c r="T2" s="30"/>
       <c r="U2" s="30"/>
       <c r="V2" s="30" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="W2" s="30"/>
       <c r="X2" s="19"/>
@@ -1147,10 +1144,10 @@
     <row r="4" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>4</v>
@@ -1214,15 +1211,15 @@
       </c>
       <c r="X4" s="20"/>
       <c r="Z4" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AA4" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="4"/>
       <c r="AD4" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AE4" s="8"/>
       <c r="AF4" s="8"/>
@@ -1233,10 +1230,10 @@
     <row r="5" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>4</v>
@@ -1274,15 +1271,15 @@
       <c r="W5" s="24"/>
       <c r="X5" s="20"/>
       <c r="Z5" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
@@ -1293,10 +1290,10 @@
     <row r="6" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="24"/>
@@ -1319,20 +1316,20 @@
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
       <c r="X6" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="Z6" s="9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>6</v>
+        <v>127</v>
       </c>
       <c r="AB6" s="1"/>
       <c r="AC6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="AD6" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
@@ -1343,10 +1340,10 @@
     <row r="7" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="27"/>
@@ -1369,13 +1366,13 @@
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
       <c r="X7" s="16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
@@ -1384,10 +1381,10 @@
     <row r="8" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="27"/>
@@ -1410,13 +1407,13 @@
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
       <c r="X8" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>8</v>
+        <v>127</v>
       </c>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
@@ -1425,10 +1422,10 @@
     <row r="9" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="27"/>
@@ -1451,16 +1448,16 @@
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
       <c r="X9" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -1483,16 +1480,16 @@
       <c r="V10" s="24"/>
       <c r="W10" s="24"/>
       <c r="X10" s="16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -1515,16 +1512,16 @@
       <c r="V11" s="24"/>
       <c r="W11" s="24"/>
       <c r="X11" s="16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
@@ -1547,16 +1544,16 @@
       <c r="V12" s="24"/>
       <c r="W12" s="24"/>
       <c r="X12" s="16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
@@ -1579,17 +1576,17 @@
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
       <c r="X13" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Z13" s="16"/>
     </row>
     <row r="14" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
@@ -1612,16 +1609,16 @@
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
       <c r="X14" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
@@ -1644,16 +1641,16 @@
       <c r="V15" s="24"/>
       <c r="W15" s="24"/>
       <c r="X15" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
@@ -1676,16 +1673,16 @@
       <c r="V16" s="24"/>
       <c r="W16" s="24"/>
       <c r="X16" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
@@ -1708,16 +1705,16 @@
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
       <c r="X17" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
@@ -1744,10 +1741,10 @@
     <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="24"/>
@@ -1770,16 +1767,16 @@
       <c r="V19" s="24"/>
       <c r="W19" s="24"/>
       <c r="X19" s="16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="27"/>
@@ -1802,16 +1799,16 @@
       <c r="V20" s="24"/>
       <c r="W20" s="24"/>
       <c r="X20" s="16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
@@ -1834,16 +1831,16 @@
       <c r="V21" s="24"/>
       <c r="W21" s="24"/>
       <c r="X21" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
@@ -1866,16 +1863,16 @@
       <c r="V22" s="24"/>
       <c r="W22" s="24"/>
       <c r="X22" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
@@ -1898,16 +1895,16 @@
       <c r="V23" s="24"/>
       <c r="W23" s="24"/>
       <c r="X23" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
@@ -1930,16 +1927,16 @@
       <c r="V24" s="24"/>
       <c r="W24" s="24"/>
       <c r="X24" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
@@ -1947,7 +1944,7 @@
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
-      <c r="J25" s="27"/>
+      <c r="J25" s="26"/>
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
@@ -1962,16 +1959,16 @@
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
       <c r="X25" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
@@ -1994,16 +1991,16 @@
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
       <c r="X26" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
@@ -2026,16 +2023,16 @@
       <c r="V27" s="24"/>
       <c r="W27" s="24"/>
       <c r="X27" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
@@ -2058,16 +2055,16 @@
       <c r="V28" s="24"/>
       <c r="W28" s="24"/>
       <c r="X28" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
@@ -2090,16 +2087,16 @@
       <c r="V29" s="24"/>
       <c r="W29" s="24"/>
       <c r="X29" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
@@ -2122,16 +2119,16 @@
       <c r="V30" s="24"/>
       <c r="W30" s="24"/>
       <c r="X30" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
@@ -2154,16 +2151,16 @@
       <c r="V31" s="24"/>
       <c r="W31" s="24"/>
       <c r="X31" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
@@ -2186,16 +2183,16 @@
       <c r="V32" s="24"/>
       <c r="W32" s="24"/>
       <c r="X32" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D33" s="24"/>
       <c r="E33" s="24"/>
@@ -2218,16 +2215,16 @@
       <c r="V33" s="24"/>
       <c r="W33" s="24"/>
       <c r="X33" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
@@ -2250,16 +2247,16 @@
       <c r="V34" s="24"/>
       <c r="W34" s="24"/>
       <c r="X34" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
@@ -2282,16 +2279,16 @@
       <c r="V35" s="24"/>
       <c r="W35" s="24"/>
       <c r="X35" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -2314,16 +2311,16 @@
       <c r="V36" s="24"/>
       <c r="W36" s="24"/>
       <c r="X36" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
@@ -2346,16 +2343,16 @@
       <c r="V37" s="26"/>
       <c r="W37" s="24"/>
       <c r="X37" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
@@ -2382,10 +2379,10 @@
     <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
@@ -2408,16 +2405,16 @@
       <c r="V39" s="24"/>
       <c r="W39" s="24"/>
       <c r="X39" s="16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
@@ -2440,16 +2437,16 @@
       <c r="V40" s="24"/>
       <c r="W40" s="24"/>
       <c r="X40" s="16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D41" s="24"/>
       <c r="E41" s="24"/>
@@ -2472,16 +2469,16 @@
       <c r="V41" s="24"/>
       <c r="W41" s="24"/>
       <c r="X41" s="16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D42" s="24"/>
       <c r="E42" s="24"/>
@@ -2504,16 +2501,16 @@
       <c r="V42" s="24"/>
       <c r="W42" s="24"/>
       <c r="X42" s="16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
@@ -2548,10 +2545,10 @@
     <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D44" s="24"/>
       <c r="E44" s="24"/>
@@ -2586,10 +2583,10 @@
     <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D45" s="24"/>
       <c r="E45" s="24"/>
@@ -2612,16 +2609,16 @@
       <c r="V45" s="24"/>
       <c r="W45" s="24"/>
       <c r="X45" s="16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D46" s="24"/>
       <c r="E46" s="24"/>
@@ -2644,16 +2641,16 @@
       <c r="V46" s="24"/>
       <c r="W46" s="24"/>
       <c r="X46" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="24"/>
@@ -2676,16 +2673,16 @@
       <c r="V47" s="24"/>
       <c r="W47" s="24"/>
       <c r="X47" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
@@ -2708,16 +2705,16 @@
       <c r="V48" s="24"/>
       <c r="W48" s="24"/>
       <c r="X48" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="24"/>
@@ -2740,16 +2737,16 @@
       <c r="V49" s="24"/>
       <c r="W49" s="24"/>
       <c r="X49" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="24"/>
@@ -2780,10 +2777,10 @@
     <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D51" s="24"/>
       <c r="E51" s="24"/>
@@ -2806,16 +2803,16 @@
       <c r="V51" s="24"/>
       <c r="W51" s="24"/>
       <c r="X51" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D52" s="24"/>
       <c r="E52" s="24"/>
@@ -2838,16 +2835,16 @@
       <c r="V52" s="24"/>
       <c r="W52" s="24"/>
       <c r="X52" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
@@ -2878,10 +2875,10 @@
     <row r="54" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D54" s="24"/>
       <c r="E54" s="24"/>
@@ -2904,16 +2901,16 @@
       <c r="V54" s="24"/>
       <c r="W54" s="24"/>
       <c r="X54" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D55" s="24"/>
       <c r="E55" s="24"/>
@@ -2936,16 +2933,16 @@
       <c r="V55" s="24"/>
       <c r="W55" s="24"/>
       <c r="X55" s="16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D56" s="24"/>
       <c r="E56" s="24"/>
@@ -2990,10 +2987,10 @@
     <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D57" s="24"/>
       <c r="E57" s="24"/>
@@ -3032,10 +3029,10 @@
     <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D58" s="24"/>
       <c r="E58" s="24"/>
@@ -3058,16 +3055,16 @@
       <c r="V58" s="24"/>
       <c r="W58" s="24"/>
       <c r="X58" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D59" s="24"/>
       <c r="E59" s="24"/>
@@ -3090,16 +3087,16 @@
       <c r="V59" s="24"/>
       <c r="W59" s="24"/>
       <c r="X59" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D60" s="24"/>
       <c r="E60" s="24"/>
@@ -3122,16 +3119,16 @@
       <c r="V60" s="24"/>
       <c r="W60" s="24"/>
       <c r="X60" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D61" s="24"/>
       <c r="E61" s="24"/>
@@ -3154,16 +3151,16 @@
       <c r="V61" s="24"/>
       <c r="W61" s="24"/>
       <c r="X61" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D62" s="24"/>
       <c r="E62" s="24"/>
@@ -3186,16 +3183,16 @@
       <c r="V62" s="24"/>
       <c r="W62" s="24"/>
       <c r="X62" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D63" s="24"/>
       <c r="E63" s="24"/>
@@ -3230,10 +3227,10 @@
     <row r="64" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D64" s="24"/>
       <c r="E64" s="24"/>
@@ -3256,16 +3253,16 @@
       <c r="V64" s="24"/>
       <c r="W64" s="24"/>
       <c r="X64" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D65" s="24"/>
       <c r="E65" s="24"/>
@@ -3288,16 +3285,16 @@
       <c r="V65" s="24"/>
       <c r="W65" s="24"/>
       <c r="X65" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D66" s="24"/>
       <c r="E66" s="24"/>
@@ -3320,16 +3317,16 @@
       <c r="V66" s="24"/>
       <c r="W66" s="24"/>
       <c r="X66" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D67" s="24"/>
       <c r="E67" s="24"/>
@@ -3352,16 +3349,16 @@
       <c r="V67" s="24"/>
       <c r="W67" s="24"/>
       <c r="X67" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D68" s="24"/>
       <c r="E68" s="24"/>
@@ -3384,16 +3381,16 @@
       <c r="V68" s="24"/>
       <c r="W68" s="24"/>
       <c r="X68" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D69" s="24"/>
       <c r="E69" s="24"/>
@@ -3424,10 +3421,10 @@
     <row r="70" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D70" s="24"/>
       <c r="E70" s="24"/>
@@ -3450,16 +3447,16 @@
       <c r="V70" s="24"/>
       <c r="W70" s="24"/>
       <c r="X70" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D71" s="24"/>
       <c r="E71" s="24"/>
@@ -3482,16 +3479,16 @@
       <c r="V71" s="24"/>
       <c r="W71" s="24"/>
       <c r="X71" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D72" s="24"/>
       <c r="E72" s="24"/>
@@ -3514,16 +3511,16 @@
       <c r="V72" s="24"/>
       <c r="W72" s="24"/>
       <c r="X72" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D73" s="24"/>
       <c r="E73" s="24"/>
@@ -3564,10 +3561,10 @@
     <row r="74" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D74" s="24"/>
       <c r="E74" s="24"/>
@@ -3608,10 +3605,10 @@
     <row r="75" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D75" s="24"/>
       <c r="E75" s="24"/>
@@ -3634,16 +3631,16 @@
       <c r="V75" s="24"/>
       <c r="W75" s="24"/>
       <c r="X75" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D76" s="24"/>
       <c r="E76" s="24"/>
@@ -3666,16 +3663,16 @@
       <c r="V76" s="24"/>
       <c r="W76" s="24"/>
       <c r="X76" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D77" s="24"/>
       <c r="E77" s="24"/>
@@ -3698,16 +3695,16 @@
       <c r="V77" s="24"/>
       <c r="W77" s="24"/>
       <c r="X77" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D78" s="24"/>
       <c r="E78" s="24"/>
@@ -3730,16 +3727,16 @@
       <c r="V78" s="24"/>
       <c r="W78" s="24"/>
       <c r="X78" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D79" s="24"/>
       <c r="E79" s="24"/>
@@ -3762,16 +3759,16 @@
       <c r="V79" s="24"/>
       <c r="W79" s="24"/>
       <c r="X79" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D80" s="24"/>
       <c r="E80" s="24"/>
@@ -3794,16 +3791,16 @@
       <c r="V80" s="24"/>
       <c r="W80" s="24"/>
       <c r="X80" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="81" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D81" s="24"/>
       <c r="E81" s="24"/>
@@ -3826,16 +3823,16 @@
       <c r="V81" s="24"/>
       <c r="W81" s="24"/>
       <c r="X81" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D82" s="24"/>
       <c r="E82" s="24"/>
@@ -3858,16 +3855,16 @@
       <c r="V82" s="24"/>
       <c r="W82" s="24"/>
       <c r="X82" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D83" s="24"/>
       <c r="E83" s="24"/>
@@ -3890,16 +3887,16 @@
       <c r="V83" s="24"/>
       <c r="W83" s="24"/>
       <c r="X83" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D84" s="24"/>
       <c r="E84" s="24"/>
@@ -3922,16 +3919,16 @@
       <c r="V84" s="24"/>
       <c r="W84" s="24"/>
       <c r="X84" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D85" s="24"/>
       <c r="E85" s="24"/>
@@ -3954,16 +3951,16 @@
       <c r="V85" s="24"/>
       <c r="W85" s="24"/>
       <c r="X85" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D86" s="24"/>
       <c r="E86" s="24"/>
@@ -3986,16 +3983,16 @@
       <c r="V86" s="24"/>
       <c r="W86" s="24"/>
       <c r="X86" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D87" s="24"/>
       <c r="E87" s="24"/>
@@ -4018,16 +4015,16 @@
       <c r="V87" s="24"/>
       <c r="W87" s="24"/>
       <c r="X87" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D88" s="24"/>
       <c r="E88" s="24"/>
@@ -4050,16 +4047,16 @@
       <c r="V88" s="24"/>
       <c r="W88" s="24"/>
       <c r="X88" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D89" s="24"/>
       <c r="E89" s="24"/>
@@ -4096,10 +4093,10 @@
     <row r="90" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D90" s="24"/>
       <c r="E90" s="24"/>
@@ -4122,16 +4119,16 @@
       <c r="V90" s="24"/>
       <c r="W90" s="24"/>
       <c r="X90" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C91" s="18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D91" s="24"/>
       <c r="E91" s="24"/>
@@ -4154,16 +4151,16 @@
       <c r="V91" s="24"/>
       <c r="W91" s="24"/>
       <c r="X91" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D92" s="24"/>
       <c r="E92" s="24"/>
@@ -4186,16 +4183,16 @@
       <c r="V92" s="24"/>
       <c r="W92" s="24"/>
       <c r="X92" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="93" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D93" s="24"/>
       <c r="E93" s="24"/>
@@ -4218,16 +4215,16 @@
       <c r="V93" s="24"/>
       <c r="W93" s="24"/>
       <c r="X93" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="94" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D94" s="24"/>
       <c r="E94" s="24"/>
@@ -4250,16 +4247,16 @@
       <c r="V94" s="24"/>
       <c r="W94" s="24"/>
       <c r="X94" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C95" s="18" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D95" s="24"/>
       <c r="E95" s="24"/>
@@ -4282,16 +4279,16 @@
       <c r="V95" s="24"/>
       <c r="W95" s="24"/>
       <c r="X95" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D96" s="24"/>
       <c r="E96" s="24"/>
@@ -4314,16 +4311,16 @@
       <c r="V96" s="24"/>
       <c r="W96" s="24"/>
       <c r="X96" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="97" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D97" s="24"/>
       <c r="E97" s="24"/>
@@ -4346,16 +4343,16 @@
       <c r="V97" s="24"/>
       <c r="W97" s="24"/>
       <c r="X97" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="98" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D98" s="24"/>
       <c r="E98" s="24"/>
@@ -4378,16 +4375,16 @@
       <c r="V98" s="24"/>
       <c r="W98" s="24"/>
       <c r="X98" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="99" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D99" s="24"/>
       <c r="E99" s="24"/>
@@ -4428,10 +4425,10 @@
     <row r="100" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D100" s="24"/>
       <c r="E100" s="24"/>
@@ -4454,16 +4451,16 @@
       <c r="V100" s="24"/>
       <c r="W100" s="24"/>
       <c r="X100" s="16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="101" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D101" s="24"/>
       <c r="E101" s="24"/>
@@ -4486,16 +4483,16 @@
       <c r="V101" s="24"/>
       <c r="W101" s="24"/>
       <c r="X101" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D102" s="24"/>
       <c r="E102" s="24"/>
@@ -4536,10 +4533,10 @@
     <row r="103" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D103" s="24"/>
       <c r="E103" s="24"/>
@@ -4570,10 +4567,10 @@
     <row r="104" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D104" s="24"/>
       <c r="E104" s="24"/>
@@ -4596,16 +4593,16 @@
       <c r="V104" s="24"/>
       <c r="W104" s="24"/>
       <c r="X104" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="105" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D105" s="24"/>
       <c r="E105" s="24"/>
@@ -4628,16 +4625,16 @@
       <c r="V105" s="24"/>
       <c r="W105" s="24"/>
       <c r="X105" s="16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D106" s="24"/>
       <c r="E106" s="24"/>
@@ -4660,16 +4657,16 @@
       <c r="V106" s="24"/>
       <c r="W106" s="24"/>
       <c r="X106" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="107" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C107" s="18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D107" s="24"/>
       <c r="E107" s="24"/>
@@ -4692,16 +4689,16 @@
       <c r="V107" s="24"/>
       <c r="W107" s="24"/>
       <c r="X107" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D108" s="24"/>
       <c r="E108" s="24"/>
@@ -4734,10 +4731,10 @@
     <row r="109" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D109" s="24"/>
       <c r="E109" s="24"/>
@@ -4760,16 +4757,16 @@
       <c r="V109" s="24"/>
       <c r="W109" s="24"/>
       <c r="X109" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D110" s="24"/>
       <c r="E110" s="24"/>
@@ -4792,16 +4789,16 @@
       <c r="V110" s="24"/>
       <c r="W110" s="24"/>
       <c r="X110" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="111" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D111" s="24"/>
       <c r="E111" s="24"/>
@@ -4824,16 +4821,16 @@
       <c r="V111" s="24"/>
       <c r="W111" s="24"/>
       <c r="X111" s="16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="112" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D112" s="24"/>
       <c r="E112" s="24"/>
@@ -4866,10 +4863,10 @@
     <row r="113" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D113" s="24"/>
       <c r="E113" s="24"/>
@@ -4892,7 +4889,7 @@
       <c r="V113" s="26"/>
       <c r="W113" s="26"/>
       <c r="X113" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="114" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>